<commit_message>
First test complete - QA pending
</commit_message>
<xml_diff>
--- a/Phase 2 Workflow/WE_treatment_dummy.xlsx
+++ b/Phase 2 Workflow/WE_treatment_dummy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://humberital-my.sharepoint.com/personal/n01609495_humber_ca/Documents/Desktop/LLM_Resume_EDA_and_Parsing/Phase 2 Workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048097958506E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95745E2D-4582-42A3-9DD9-8D814AC932CA}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC1048097958506E5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6C0653C-61DA-4DC4-AF11-30D9647C8643}"/>
   <bookViews>
     <workbookView xWindow="51720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>title</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Collaborated with cross</t>
-  </si>
-  <si>
-    <t>functional teams</t>
   </si>
   <si>
     <t xml:space="preserve"> Built RESTful APIs using Flask</t>
@@ -208,6 +205,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -484,7 +485,7 @@
     <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,16 +505,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,11 +542,8 @@
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -565,16 +563,16 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -594,16 +592,16 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -623,16 +621,16 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -652,13 +650,13 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>